<commit_message>
corrected bugs on output of publications
</commit_message>
<xml_diff>
--- a/Data_files/publications.xlsx
+++ b/Data_files/publications.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="28020" windowHeight="16920"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="28020" windowHeight="16920" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Editorial Material" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="752">
   <si>
     <t>Year</t>
   </si>
@@ -2394,8 +2394,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2413,11 +2415,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2719,8 +2723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2792,8 +2796,17 @@
       <c r="H2" t="s">
         <v>616</v>
       </c>
+      <c r="I2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J2" t="s">
+        <v>616</v>
+      </c>
       <c r="K2" t="s">
         <v>484</v>
+      </c>
+      <c r="L2" t="s">
+        <v>616</v>
       </c>
       <c r="M2" t="s">
         <v>561</v>
@@ -2825,7 +2838,16 @@
       <c r="H3" t="s">
         <v>616</v>
       </c>
+      <c r="I3" t="s">
+        <v>616</v>
+      </c>
+      <c r="J3" t="s">
+        <v>616</v>
+      </c>
       <c r="K3" t="s">
+        <v>616</v>
+      </c>
+      <c r="L3" t="s">
         <v>616</v>
       </c>
       <c r="M3" s="3" t="s">
@@ -2858,8 +2880,17 @@
       <c r="H4" t="s">
         <v>618</v>
       </c>
+      <c r="I4" t="s">
+        <v>616</v>
+      </c>
+      <c r="J4" t="s">
+        <v>616</v>
+      </c>
       <c r="K4" t="s">
         <v>461</v>
+      </c>
+      <c r="L4" t="s">
+        <v>616</v>
       </c>
       <c r="M4" t="s">
         <v>550</v>
@@ -2891,8 +2922,17 @@
       <c r="H5" t="s">
         <v>616</v>
       </c>
+      <c r="I5" t="s">
+        <v>616</v>
+      </c>
+      <c r="J5" t="s">
+        <v>616</v>
+      </c>
       <c r="K5" t="s">
         <v>210</v>
+      </c>
+      <c r="L5" t="s">
+        <v>616</v>
       </c>
       <c r="M5" t="s">
         <v>736</v>
@@ -2924,8 +2964,17 @@
       <c r="H6" t="s">
         <v>616</v>
       </c>
+      <c r="I6" t="s">
+        <v>616</v>
+      </c>
+      <c r="J6" t="s">
+        <v>616</v>
+      </c>
       <c r="K6" t="s">
         <v>468</v>
+      </c>
+      <c r="L6" t="s">
+        <v>616</v>
       </c>
       <c r="M6" t="s">
         <v>552</v>
@@ -2957,8 +3006,17 @@
       <c r="H7" t="s">
         <v>618</v>
       </c>
+      <c r="I7" t="s">
+        <v>616</v>
+      </c>
+      <c r="J7" t="s">
+        <v>616</v>
+      </c>
       <c r="K7" t="s">
         <v>216</v>
+      </c>
+      <c r="L7" t="s">
+        <v>616</v>
       </c>
       <c r="M7" t="s">
         <v>546</v>
@@ -2990,8 +3048,17 @@
       <c r="H8" t="s">
         <v>616</v>
       </c>
+      <c r="I8" t="s">
+        <v>616</v>
+      </c>
+      <c r="J8" t="s">
+        <v>616</v>
+      </c>
       <c r="K8" t="s">
         <v>473</v>
+      </c>
+      <c r="L8" t="s">
+        <v>616</v>
       </c>
       <c r="M8" t="s">
         <v>550</v>
@@ -3023,8 +3090,17 @@
       <c r="H9" t="s">
         <v>616</v>
       </c>
+      <c r="I9" t="s">
+        <v>616</v>
+      </c>
+      <c r="J9" t="s">
+        <v>616</v>
+      </c>
       <c r="K9" t="s">
         <v>467</v>
+      </c>
+      <c r="L9" t="s">
+        <v>616</v>
       </c>
       <c r="M9" t="s">
         <v>737</v>
@@ -3056,7 +3132,16 @@
       <c r="H10" t="s">
         <v>616</v>
       </c>
+      <c r="I10" t="s">
+        <v>616</v>
+      </c>
+      <c r="J10" t="s">
+        <v>616</v>
+      </c>
       <c r="K10" t="s">
+        <v>616</v>
+      </c>
+      <c r="L10" t="s">
         <v>616</v>
       </c>
       <c r="M10" t="s">
@@ -3089,8 +3174,17 @@
       <c r="H11" t="s">
         <v>616</v>
       </c>
+      <c r="I11" t="s">
+        <v>616</v>
+      </c>
+      <c r="J11" t="s">
+        <v>616</v>
+      </c>
       <c r="K11" t="s">
         <v>461</v>
+      </c>
+      <c r="L11" t="s">
+        <v>616</v>
       </c>
       <c r="M11" t="s">
         <v>525</v>
@@ -3122,7 +3216,16 @@
       <c r="H12" t="s">
         <v>616</v>
       </c>
+      <c r="I12" t="s">
+        <v>616</v>
+      </c>
+      <c r="J12" t="s">
+        <v>616</v>
+      </c>
       <c r="K12" t="s">
+        <v>616</v>
+      </c>
+      <c r="L12" t="s">
         <v>616</v>
       </c>
       <c r="M12" t="s">
@@ -3135,6 +3238,7 @@
     <sortCondition ref="L2:L12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3143,7 +3247,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:L1"/>
+      <selection activeCell="L2" sqref="L2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3216,9 +3320,16 @@
       <c r="H2" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K2" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>616</v>
       </c>
       <c r="M2" t="s">
@@ -3251,8 +3362,17 @@
       <c r="H3" t="s">
         <v>616</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K3" t="s">
         <v>492</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>616</v>
       </c>
       <c r="M3" t="s">
         <v>577</v>
@@ -3284,8 +3404,17 @@
       <c r="H4" t="s">
         <v>616</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K4" t="s">
         <v>491</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>616</v>
       </c>
       <c r="M4" t="s">
         <v>575</v>
@@ -3317,10 +3446,17 @@
       <c r="H5" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K5" t="s">
         <v>490</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>616</v>
       </c>
       <c r="M5" t="s">
         <v>574</v>
@@ -3352,8 +3488,17 @@
       <c r="H6" t="s">
         <v>616</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K6" t="s">
         <v>480</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>616</v>
       </c>
       <c r="M6" t="s">
         <v>567</v>
@@ -3385,8 +3530,17 @@
       <c r="H7" t="s">
         <v>616</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K7" t="s">
         <v>481</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>616</v>
       </c>
       <c r="M7" t="s">
         <v>561</v>
@@ -3405,7 +3559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:L1"/>
     </sheetView>
   </sheetViews>
@@ -8465,8 +8619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>